<commit_message>
Report is added, transformer parameters are recalculated.
</commit_message>
<xml_diff>
--- a/Project 1/Inductor Design_CA.xlsx
+++ b/Project 1/Inductor Design_CA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>B_ac_max(T)</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Permeance (Wb/A-t)</t>
-  </si>
-  <si>
-    <t>B_mean(T)</t>
   </si>
   <si>
     <t>Datasheet_values</t>
@@ -548,7 +545,7 @@
   <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C18" sqref="C18:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +638,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>15</v>
@@ -677,10 +674,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <f>((Q4*R4*D4*E4)/(O4*10^-3))</f>
@@ -737,10 +734,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C5" s="3">
         <f>((Q5*R5*D5*E5)/(O5*10^-3))</f>
@@ -797,7 +794,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3">
         <f>((Q6*R6*D6*E6)/(O6*10^-3))</f>
@@ -854,7 +851,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3">
         <f>(D7*E7)/(G7*N7*10^-6)</f>
@@ -911,7 +908,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3">
         <f>(D8*E8)/(G8*N8*10^-6)</f>
@@ -1113,28 +1110,12 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="3">
-        <f t="shared" ref="C18:C25" si="0">((Q18*R18*D18*E18)/(O18*10^-3))</f>
-        <v>0.27796580160794482</v>
-      </c>
-      <c r="D18" s="3">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" ref="F18:F25" si="1">1/G18</f>
-        <v>2.3800821762680275E-6</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" ref="G18:G25" si="2">(O18*10^-3)/(Q18*R18*N18*10^-6)</f>
-        <v>420153.56023042934</v>
-      </c>
-      <c r="H18" s="3">
-        <f t="shared" ref="H18:H25" si="3">((D18*D18)/G18)/10^-3</f>
-        <v>0.15232525928115376</v>
-      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1151,34 +1132,18 @@
         <v>3000</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" ref="R18:R25" si="4">4*PI()*10^(-7)</f>
+        <f t="shared" ref="R18:R25" si="0">4*PI()*10^(-7)</f>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.29139410120253156</v>
-      </c>
-      <c r="D19" s="3">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" si="1"/>
-        <v>2.4950619915466763E-6</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="2"/>
-        <v>400791.64501243719</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="3"/>
-        <v>0.15968396745898727</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1195,34 +1160,18 @@
         <v>3000</v>
       </c>
       <c r="R19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
-      <c r="C20" s="3">
-        <f t="shared" si="0"/>
-        <v>0.30618567994377682</v>
-      </c>
-      <c r="D20" s="3">
-        <v>8</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F20" s="3">
-        <f t="shared" si="1"/>
-        <v>2.6217148845185887E-6</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="2"/>
-        <v>381429.72979444504</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" si="3"/>
-        <v>0.16778975260918969</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1239,34 +1188,18 @@
         <v>3000</v>
       </c>
       <c r="R20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
-      <c r="C21" s="3">
-        <f t="shared" si="0"/>
-        <v>0.32255924571617128</v>
-      </c>
-      <c r="D21" s="3">
-        <v>8</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7619135414447161E-6</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="2"/>
-        <v>362067.81457645295</v>
-      </c>
-      <c r="H21" s="3">
-        <f t="shared" si="3"/>
-        <v>0.17676246665246181</v>
-      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1283,34 +1216,18 @@
         <v>3000</v>
       </c>
       <c r="R21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
-      <c r="C22" s="3">
-        <f t="shared" si="0"/>
-        <v>0.25450877193638832</v>
-      </c>
-      <c r="D22" s="3">
-        <v>8</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="1"/>
-        <v>2.1792313597053249E-6</v>
-      </c>
-      <c r="G22" s="3">
-        <f t="shared" si="2"/>
-        <v>458877.39066641359</v>
-      </c>
-      <c r="H22" s="3">
-        <f t="shared" si="3"/>
-        <v>0.13947080702114079</v>
-      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1327,34 +1244,18 @@
         <v>3000</v>
       </c>
       <c r="R22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
-      <c r="C23" s="3">
-        <f t="shared" si="0"/>
-        <v>0.24420477307256694</v>
-      </c>
-      <c r="D23" s="3">
-        <v>8</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0910033694338539E-6</v>
-      </c>
-      <c r="G23" s="3">
-        <f t="shared" si="2"/>
-        <v>478239.30588440574</v>
-      </c>
-      <c r="H23" s="3">
-        <f t="shared" si="3"/>
-        <v>0.13382421564376665</v>
-      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1371,34 +1272,18 @@
         <v>3000</v>
       </c>
       <c r="R23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
-      <c r="C24" s="3">
-        <f t="shared" si="0"/>
-        <v>0.23470264182460712</v>
-      </c>
-      <c r="D24" s="3">
-        <v>8</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0096413706231983E-6</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" si="2"/>
-        <v>497601.22110239789</v>
-      </c>
-      <c r="H24" s="3">
-        <f t="shared" si="3"/>
-        <v>0.12861704771988469</v>
-      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1415,34 +1300,18 @@
         <v>3000</v>
       </c>
       <c r="R24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
-      <c r="C25" s="3">
-        <f t="shared" si="0"/>
-        <v>0.22591228070758063</v>
-      </c>
-      <c r="D25" s="3">
-        <v>8</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="1"/>
-        <v>1.9343739035586588E-6</v>
-      </c>
-      <c r="G25" s="3">
-        <f t="shared" si="2"/>
-        <v>516963.13632039004</v>
-      </c>
-      <c r="H25" s="3">
-        <f t="shared" si="3"/>
-        <v>0.12379992982775416</v>
-      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1459,7 +1328,7 @@
         <v>3000</v>
       </c>
       <c r="R25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
@@ -1503,13 +1372,9 @@
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
-      <c r="C28" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="C28" s="6"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1526,18 +1391,9 @@
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="3">
-        <f>AVERAGE(C4:C25)</f>
-        <v>0.23441430947432834</v>
-      </c>
-      <c r="D29" s="3">
-        <f>(D25*E25)/(C29*13.7*10^-6)</f>
-        <v>498213.27644110046</v>
-      </c>
-      <c r="E29" s="3">
-        <f>(100/D29)/10^-3</f>
-        <v>0.20071725248739361</v>
-      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>

</xml_diff>